<commit_message>
changre pi to PI
</commit_message>
<xml_diff>
--- a/inline_double_plunger_01.xlsx
+++ b/inline_double_plunger_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kutlayhanli/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27095F03-B280-0F4A-8530-DCFD77739E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D5F7977-C8D9-7D43-8149-219D9B23B62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <t>goal_A</t>
   </si>
   <si>
-    <t>pi * goal_r^2</t>
+    <t>PI * goal_r^2</t>
   </si>
   <si>
     <t>m*m</t>
@@ -78,7 +78,7 @@
     <t>main_boss_A</t>
   </si>
   <si>
-    <t>pi*main_boss_inner_r^2</t>
+    <t>PI*main_boss_inner_r^2</t>
   </si>
   <si>
     <t>outlet_orifice_A</t>
@@ -90,7 +90,7 @@
     <t>outlet_orifice_r</t>
   </si>
   <si>
-    <t>sqrt(outlet_orifice_A/pi)</t>
+    <t>sqrt(outlet_orifice_A/PI)</t>
   </si>
   <si>
     <t>outlet_entrance_A</t>
@@ -102,7 +102,7 @@
     <t>outlet_entrance_r</t>
   </si>
   <si>
-    <t>sqrt(outlet_entrance_A/pi)</t>
+    <t>sqrt(outlet_entrance_A/PI)</t>
   </si>
   <si>
     <t>outlet_boss_t</t>
@@ -120,7 +120,7 @@
     <t>outlet_boss_A</t>
   </si>
   <si>
-    <t>pi*outlet_boss_r^2</t>
+    <t>PI*outlet_boss_r^2</t>
   </si>
   <si>
     <t>main_A</t>
@@ -132,13 +132,13 @@
     <t>main_r</t>
   </si>
   <si>
-    <t>sqrt(main_A/pi)</t>
+    <t>sqrt(main_A/PI)</t>
   </si>
   <si>
     <t>main_high_pressure_A</t>
   </si>
   <si>
-    <t>pi * (main_r^2 - outlet_boss_r^2)</t>
+    <t>PI * (main_r^2 - outlet_boss_r^2)</t>
   </si>
   <si>
     <t>main_down_side_A</t>
@@ -153,7 +153,7 @@
     <t>main_boss_out_r</t>
   </si>
   <si>
-    <t>sqrt(main_low_pressure_A/pi)</t>
+    <t>sqrt(main_low_pressure_A/PI)</t>
   </si>
   <si>
     <t>3*0.001</t>
@@ -171,7 +171,7 @@
     <t>main_movement_range</t>
   </si>
   <si>
-    <t>outlet_entrance_A / (2 * pi * outlet_entrance_r)</t>
+    <t>outlet_entrance_A / (2 * PI * outlet_entrance_r)</t>
   </si>
   <si>
     <t>retainer_main_groove_depth</t>
@@ -198,34 +198,34 @@
     <t>retainer_main_boss_groove_r</t>
   </si>
   <si>
-    <t>pilot_seal_r</t>
+    <t>PIlot_seal_r</t>
   </si>
   <si>
     <t>main_boss_inner_r * 0.5</t>
   </si>
   <si>
-    <t>pilot_seal_t</t>
-  </si>
-  <si>
-    <t>pilot_stem_r</t>
-  </si>
-  <si>
-    <t>pilot_seal_r * 0.25</t>
-  </si>
-  <si>
-    <t>pilot_steam_A</t>
-  </si>
-  <si>
-    <t>pilot_stem_r^2 * pi</t>
-  </si>
-  <si>
-    <t>pilot_seal_A</t>
-  </si>
-  <si>
-    <t>pilot_seal_r^2 * pi</t>
-  </si>
-  <si>
-    <t>pilot_movement_range</t>
+    <t>PIlot_seal_t</t>
+  </si>
+  <si>
+    <t>PIlot_stem_r</t>
+  </si>
+  <si>
+    <t>PIlot_seal_r * 0.25</t>
+  </si>
+  <si>
+    <t>PIlot_steam_A</t>
+  </si>
+  <si>
+    <t>PIlot_stem_r^2 * PI</t>
+  </si>
+  <si>
+    <t>PIlot_seal_A</t>
+  </si>
+  <si>
+    <t>PIlot_seal_r^2 * PI</t>
+  </si>
+  <si>
+    <t>PIlot_movement_range</t>
   </si>
   <si>
     <t>20*0.001</t>
@@ -234,7 +234,7 @@
     <t>main_boss_h</t>
   </si>
   <si>
-    <t>pilot_movement_range * 1.05</t>
+    <t>PIlot_movement_range * 1.05</t>
   </si>
   <si>
     <t>retainer_main_boss_groove_depth</t>
@@ -270,7 +270,7 @@
     <t>inlet_outlet_distance</t>
   </si>
   <si>
-    <t>outlet_entrance_A / (2 * pi * retainer_main_boss_groove_r)</t>
+    <t>outlet_entrance_A / (2 * PI * retainer_main_boss_groove_r)</t>
   </si>
 </sst>
 </file>

</xml_diff>